<commit_message>
Bunch of major changes. Got relay.py working mostly. Need to make sure I can shape the data to better fit the project. New.py is just a example of some ideas.
</commit_message>
<xml_diff>
--- a/RelayList.xlsx
+++ b/RelayList.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/43fe702b05e59fa4/COSC Research/RelayData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="8_{4D78FCE7-7EF2-40ED-A735-776F8C0DD271}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CAACABEE-AF19-45A9-B571-D8295119DA4B}"/>
+  <xr:revisionPtr revIDLastSave="153" documentId="8_{4D78FCE7-7EF2-40ED-A735-776F8C0DD271}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1238B4F5-8779-4D9A-9F71-2D0141280FEF}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="1140" yWindow="1140" windowWidth="14400" windowHeight="7270" xr2:uid="{7E9A9F16-B4C4-4A4A-9DB9-C8E3F651EF53}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{7E9A9F16-B4C4-4A4A-9DB9-C8E3F651EF53}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="111">
   <si>
     <t>Relay Name</t>
   </si>
@@ -50,12 +50,6 @@
     <t>55808BA9B4228678BC1D300DF7A5479C5ED236D1</t>
   </si>
   <si>
-    <t>GeorgetownPontem</t>
-  </si>
-  <si>
-    <t>7C95AED7256E1D10D134942532CC72AD73AC1BD8</t>
-  </si>
-  <si>
     <t>0E17FCEDE80CD0F00F0C9D8D3690F0238E55ABF4</t>
   </si>
   <si>
@@ -66,13 +60,322 @@
   </si>
   <si>
     <t>494E5000BA79F0078DFA05E610911C2AC525572F</t>
+  </si>
+  <si>
+    <t>Citadel5</t>
+  </si>
+  <si>
+    <t>1F2EB70268CE9E18CE864D44D793E2091F3CE72C</t>
+  </si>
+  <si>
+    <t>TORtuga</t>
+  </si>
+  <si>
+    <t>05C32C5EE14454E0C4CD81DAE0F3DC32F729DA4B</t>
+  </si>
+  <si>
+    <t>blackfox</t>
+  </si>
+  <si>
+    <t>03D1EF3EF2BE5145150C58ACC72519DD860E61BA</t>
+  </si>
+  <si>
+    <t>Unnamed</t>
+  </si>
+  <si>
+    <t>3A04AC8969E55DF51C8D11C49ABF18A0CC847FC0</t>
+  </si>
+  <si>
+    <t>nuker</t>
+  </si>
+  <si>
+    <t>5FAE28CF4D1C520341EE104BF72516F4308B9485</t>
+  </si>
+  <si>
+    <t>JustExiting</t>
+  </si>
+  <si>
+    <t>2B4D5AA9997D4DDFF02BC52E173CF0C8FFFD1B9C</t>
+  </si>
+  <si>
+    <t>Exit</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>fiedlerexitrelay</t>
+  </si>
+  <si>
+    <t>09A5115DDD6179B339AD7D1930BAA1DE1F2DF61E</t>
+  </si>
+  <si>
+    <t>torexitams01</t>
+  </si>
+  <si>
+    <t>678B3A694071537AD62723BDA96C6CF1358AE67A</t>
+  </si>
+  <si>
+    <t>0AFD832F09B6C2C9E0FE99E78B29E2ED325B0E54</t>
+  </si>
+  <si>
+    <t>torexitams00</t>
+  </si>
+  <si>
+    <t>82E2708957A41EDA0819EE1C5FFC3E2DC38B9FE9</t>
+  </si>
+  <si>
+    <t>FreeExit</t>
+  </si>
+  <si>
+    <t>DAC7BBF1F2F92E748B1EB59B950674E2C39FEA51</t>
+  </si>
+  <si>
+    <t>exit000</t>
+  </si>
+  <si>
+    <t>4637E79752D5086DD832564924DD455FC7D74683</t>
+  </si>
+  <si>
+    <t>dotsrcExit2</t>
+  </si>
+  <si>
+    <t>C0C300BC2E84A503D4F51A6AD63B3F6BF3E112C2</t>
+  </si>
+  <si>
+    <t>ExiTOR</t>
+  </si>
+  <si>
+    <t>D9C55AC5549BF4940BE0ABBBE0E34CCC8D6D06E5</t>
+  </si>
+  <si>
+    <t>NeelTorExit1E</t>
+  </si>
+  <si>
+    <t>9C94F80C7B4824F6797C76296A16CADBC2B73444</t>
+  </si>
+  <si>
+    <t>DjMiddle</t>
+  </si>
+  <si>
+    <t>467D7417FFA611BC20227FE347494CE5F61218FB</t>
+  </si>
+  <si>
+    <t>middleChildRelay</t>
+  </si>
+  <si>
+    <t>E5E2A7F7D944C37A83A668AB309E402DF3159392</t>
+  </si>
+  <si>
+    <t>acid74middleguard1</t>
+  </si>
+  <si>
+    <t>D1447A980D157D08CA2BACA015EB10B34B7719EB</t>
+  </si>
+  <si>
+    <t>GlobalEntry</t>
+  </si>
+  <si>
+    <t>240032E115DD24D7D7A2E047D35478A9B108082C</t>
+  </si>
+  <si>
+    <t>Hypervistor</t>
+  </si>
+  <si>
+    <t>F50755D5018C23F6CD115F23C95CCB2DC8B608B1</t>
+  </si>
+  <si>
+    <t>Torminator4</t>
+  </si>
+  <si>
+    <t>D78734736C4CE24BE40524BF27455A4ADB995453</t>
+  </si>
+  <si>
+    <t>raptor</t>
+  </si>
+  <si>
+    <t>558B31F1D04366194A29423BBAB09DAB21EBA4DF</t>
+  </si>
+  <si>
+    <t>gator</t>
+  </si>
+  <si>
+    <t>9F9E9B6C82FF468FC668853491EB7484C3BE3DA6</t>
+  </si>
+  <si>
+    <t>slotor01</t>
+  </si>
+  <si>
+    <t>49604A7CC7E80AB3D518AFC3E95B2EA265532719</t>
+  </si>
+  <si>
+    <t>ReacTOR</t>
+  </si>
+  <si>
+    <t>5C426791CB47BDDDD97A71EB2EFC4CCC84DEB299</t>
+  </si>
+  <si>
+    <t>TorRelay1b</t>
+  </si>
+  <si>
+    <t>1AA63474AB2277A944E452649EB19044F21314E4</t>
+  </si>
+  <si>
+    <t>TorRelay3c</t>
+  </si>
+  <si>
+    <t>D021D70CD592D1BDEFB3B1DF787746983B350FFE</t>
+  </si>
+  <si>
+    <t>TorRelay2a</t>
+  </si>
+  <si>
+    <t>78425CEF7554B252668E1CFC2E80C785633B2558</t>
+  </si>
+  <si>
+    <t>root1Moh</t>
+  </si>
+  <si>
+    <t>01B8F18C11CE2877E8190FA2C81808CD087515C0</t>
+  </si>
+  <si>
+    <t>SpookySum69694</t>
+  </si>
+  <si>
+    <t>4E1537454630C398DA0BCF3F27B52E2DB0050763</t>
+  </si>
+  <si>
+    <t>arbertDelroth</t>
+  </si>
+  <si>
+    <t>0432BEE829FCB155CE92CF418B7280F9849E12D0</t>
+  </si>
+  <si>
+    <t>sn0rlax</t>
+  </si>
+  <si>
+    <t>5C386C4F91FD616F0F60F4E6D674D9E3F192C931</t>
+  </si>
+  <si>
+    <t>Akka</t>
+  </si>
+  <si>
+    <t>56927E61B51E6F363FB55498150A6DDFCF7077F2</t>
+  </si>
+  <si>
+    <t>lancelot</t>
+  </si>
+  <si>
+    <t>0C36AE99B744E32088C9ED23D7A31F8D23AE1A58</t>
+  </si>
+  <si>
+    <t>sonrisas</t>
+  </si>
+  <si>
+    <t>32742AD57C3D243DA0713BB6DFD82118DF573D2E</t>
+  </si>
+  <si>
+    <t>Zephyrdead</t>
+  </si>
+  <si>
+    <t>340704679F46C155094816B34FF6BE491C0AA16E</t>
+  </si>
+  <si>
+    <t>bebrave</t>
+  </si>
+  <si>
+    <t>1DBEC99526501D292A58F19FF763DFBAF66A062E</t>
+  </si>
+  <si>
+    <t>Liberation</t>
+  </si>
+  <si>
+    <t>0E98EA05A6DA0FA11C0C3C32BF0D6E4F8B0D1DB8</t>
+  </si>
+  <si>
+    <t>TorScale2</t>
+  </si>
+  <si>
+    <t>56909EDCDFFC04AA38593466F51F3FB2AC63414C</t>
+  </si>
+  <si>
+    <t>galtlandeu3</t>
+  </si>
+  <si>
+    <t>133D3D8F3B7220A314BAF02A42A566E230234638</t>
+  </si>
+  <si>
+    <t>Andromeda</t>
+  </si>
+  <si>
+    <t>3D8BEC9FB68E2C7EB7BEB166E51643C43AFBCC57</t>
+  </si>
+  <si>
+    <t>TheGreatKing</t>
+  </si>
+  <si>
+    <t>0824D7C7FB117D5C6AC01581FD798E670C37C804</t>
+  </si>
+  <si>
+    <t>uneasyspeak</t>
+  </si>
+  <si>
+    <t>36F7F3BCC3847FEE902F460E6011A5627437F138</t>
+  </si>
+  <si>
+    <t>Rantallion</t>
+  </si>
+  <si>
+    <t>2CD23D10948D1C6039977852274F700278B39EE8</t>
+  </si>
+  <si>
+    <t>FatalUnicorn</t>
+  </si>
+  <si>
+    <t>5B6DAB1516F3312E7F3E8DACFAABC732A5DF67CC</t>
+  </si>
+  <si>
+    <t>MantisDance</t>
+  </si>
+  <si>
+    <t>4938A9B50436B901B355F5FD1D9D16805A4E41F8</t>
+  </si>
+  <si>
+    <t>ForPrivacyNET</t>
+  </si>
+  <si>
+    <t>24FDF4754BB3775A6D54E078DCBBCA43D7B1B07E</t>
+  </si>
+  <si>
+    <t>NTH15R2</t>
+  </si>
+  <si>
+    <t>09E5621C0D7400FC18EF137A679F7FEB78F8650C</t>
+  </si>
+  <si>
+    <t>TERMINATOR3000</t>
+  </si>
+  <si>
+    <t>4D363421C5EA94BCEFA6F29B38C9E575C7931EAD</t>
+  </si>
+  <si>
+    <t>TheJabulani</t>
+  </si>
+  <si>
+    <t>6356937B20C837B8B6427CCD7183CAAE63021CAF</t>
+  </si>
+  <si>
+    <t>ShadowTower</t>
+  </si>
+  <si>
+    <t>24BA11FA583CA9EE4C3623936B58B8870854B12F</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -91,6 +394,12 @@
       <color rgb="FF333333"/>
       <name val="Consolas"/>
       <family val="3"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
+      <name val="Source Sans Pro"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -128,7 +437,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -137,6 +446,7 @@
     <xf numFmtId="11" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -152,6 +462,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -471,10 +785,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDBA6A9F-7348-4D92-B16C-550D096F5C82}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:C55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L10" sqref="L10"/>
+    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
+      <selection activeCell="A53" sqref="A53:XFD53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -483,15 +797,18 @@
     <col min="2" max="2" width="39.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -499,31 +816,462 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    </row>
+    <row r="4" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="1" t="s">
+    </row>
+    <row r="5" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A5" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="2" t="s">
         <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A6" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A7" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A8" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A9" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A10" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A11" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A12" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A13" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C13" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A14" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C14" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A15" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C15" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A16" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C16" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A17" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C17" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A18" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C18" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A19" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C19" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A20" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A21" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A22" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A23" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A24" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A25" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A26" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A27" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A28" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A29" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A30" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A31" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A32" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A33" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A34" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A35" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A36" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A37" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A38" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A39" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A40" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A41" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A42" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A43" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A44" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A45" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A46" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A47" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A48" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A49" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A50" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A51" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A52" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="B52" s="3" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A53" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A54" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A55" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>110</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>